<commit_message>
Taxas de mortalidade + hotfix
</commit_message>
<xml_diff>
--- a/Trabalho1/Tabua_de_vida.xlsx
+++ b/Trabalho1/Tabua_de_vida.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24519"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B09B80B0-A0B6-42BA-85E4-0FB06953A622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9796592E-E97A-4A1F-AA06-6051FCCDC934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,12 +520,13 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -655,11 +656,11 @@
       </c>
       <c r="S2" s="6">
         <f t="shared" ref="S2:S17" si="2">S3+R2</f>
-        <v>9348820.3254319001</v>
+        <v>9348842.5808032155</v>
       </c>
       <c r="T2" s="1">
         <f>S2/P2</f>
-        <v>93.488203254319004</v>
+        <v>93.488425808032162</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -707,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="9">
-        <v>3.009E-4</v>
+        <v>3.0029999999999998E-4</v>
       </c>
       <c r="N3" s="1">
         <f>1.522-1.518*M2</f>
@@ -715,7 +716,7 @@
       </c>
       <c r="O3" s="1">
         <f>L3*M3/(1+(L3-N3)*M3)</f>
-        <v>1.202697858506464E-3</v>
+        <v>1.2003014513491483E-3</v>
       </c>
       <c r="P3" s="6">
         <f>P2-Q2</f>
@@ -723,19 +724,19 @@
       </c>
       <c r="Q3" s="6">
         <f>O3*P3</f>
-        <v>119.10076353217812</v>
+        <v>118.86345212420346</v>
       </c>
       <c r="R3" s="6">
         <f t="shared" si="1"/>
-        <v>494665.10409709893</v>
+        <v>494666.0533427308</v>
       </c>
       <c r="S3" s="6">
         <f t="shared" si="2"/>
-        <v>9149792.2450428605</v>
+        <v>9149814.5004141759</v>
       </c>
       <c r="T3" s="1">
         <f t="shared" ref="T3:T19" si="5">S3/P3</f>
-        <v>92.39601168399706</v>
+        <v>92.396236422165202</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -793,23 +794,23 @@
       </c>
       <c r="P4" s="6">
         <f>P3-Q3</f>
-        <v>98908.899236467827</v>
+        <v>98909.136547875794</v>
       </c>
       <c r="Q4" s="6">
         <f>O4*P4</f>
-        <v>67.581136774633023</v>
+        <v>67.581298921566656</v>
       </c>
       <c r="R4" s="6">
         <f t="shared" si="1"/>
-        <v>593117.98973493371</v>
+        <v>593119.41279264691</v>
       </c>
       <c r="S4" s="6">
         <f t="shared" si="2"/>
-        <v>8655127.1409457624</v>
+        <v>8655148.4470714442</v>
       </c>
       <c r="T4" s="1">
         <f t="shared" si="5"/>
-        <v>87.506050595643543</v>
+        <v>87.506056054609502</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -867,23 +868,23 @@
       </c>
       <c r="P5" s="6">
         <f>P4-Q4</f>
-        <v>98841.318099693191</v>
+        <v>98841.555248954232</v>
       </c>
       <c r="Q5" s="6">
         <f>O5*P5</f>
-        <v>82.152401139121309</v>
+        <v>82.152598246784351</v>
       </c>
       <c r="R5" s="6">
         <f t="shared" si="1"/>
-        <v>592639.6465924636</v>
+        <v>592641.06850249146</v>
       </c>
       <c r="S5" s="6">
         <f t="shared" si="2"/>
-        <v>8062009.1512108278</v>
+        <v>8062029.0342787979</v>
       </c>
       <c r="T5" s="1">
         <f t="shared" si="5"/>
-        <v>81.565172401680599</v>
+        <v>81.565177864439733</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -941,23 +942,23 @@
       </c>
       <c r="P6" s="6">
         <f>P5-Q5</f>
-        <v>98759.165698554076</v>
+        <v>98759.402650707445</v>
       </c>
       <c r="Q6" s="6">
         <f>O6*P6</f>
-        <v>171.49440134931444</v>
+        <v>171.49481281459367</v>
       </c>
       <c r="R6" s="6">
         <f t="shared" si="1"/>
-        <v>591700.022184578</v>
+        <v>591701.4418401717</v>
       </c>
       <c r="S6" s="6">
         <f t="shared" si="2"/>
-        <v>7469369.5046183644</v>
+        <v>7469387.9657763066</v>
       </c>
       <c r="T6" s="1">
         <f t="shared" si="5"/>
-        <v>75.63216489107829</v>
+        <v>75.632170358442337</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -1015,23 +1016,23 @@
       </c>
       <c r="P7" s="6">
         <f t="shared" ref="P7:P19" si="9">P6-Q6</f>
-        <v>98587.671297204768</v>
+        <v>98587.907837892853</v>
       </c>
       <c r="Q7" s="6">
         <f t="shared" ref="Q7:Q19" si="10">O7*P7</f>
-        <v>252.99598480668723</v>
+        <v>252.99659181812734</v>
       </c>
       <c r="R7" s="6">
         <f t="shared" si="1"/>
-        <v>590263.54785919515</v>
+        <v>590264.96406826645</v>
       </c>
       <c r="S7" s="6">
         <f t="shared" si="2"/>
-        <v>6877669.4824337866</v>
+        <v>6877686.5239361348</v>
       </c>
       <c r="T7" s="1">
         <f t="shared" si="5"/>
-        <v>69.761963052156887</v>
+        <v>69.761968529092314</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1089,23 +1090,23 @@
       </c>
       <c r="P8" s="6">
         <f t="shared" si="9"/>
-        <v>98334.675312398074</v>
+        <v>98334.911246074727</v>
       </c>
       <c r="Q8" s="6">
         <f t="shared" si="10"/>
-        <v>290.59146886099512</v>
+        <v>290.59216607500872</v>
       </c>
       <c r="R8" s="6">
         <f t="shared" si="1"/>
-        <v>588557.59453008347</v>
+        <v>588559.00664607331</v>
       </c>
       <c r="S8" s="6">
         <f t="shared" si="2"/>
-        <v>6287405.9345745919</v>
+        <v>6287421.5598678682</v>
       </c>
       <c r="T8" s="1">
         <f t="shared" si="5"/>
-        <v>63.938848779438366</v>
+        <v>63.93885427052588</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1163,23 +1164,23 @@
       </c>
       <c r="P9" s="6">
         <f t="shared" si="9"/>
-        <v>98044.083843537082</v>
+        <v>98044.319079999725</v>
       </c>
       <c r="Q9" s="6">
         <f t="shared" si="10"/>
-        <v>397.10608675245288</v>
+        <v>397.10703952622032</v>
       </c>
       <c r="R9" s="6">
         <f t="shared" si="1"/>
-        <v>586281.47262746026</v>
+        <v>586282.87928236718</v>
       </c>
       <c r="S9" s="6">
         <f t="shared" si="2"/>
-        <v>5698848.3400445087</v>
+        <v>5698862.5532217948</v>
       </c>
       <c r="T9" s="1">
         <f t="shared" si="5"/>
-        <v>58.125366841501354</v>
+        <v>58.125372348924991</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1237,23 +1238,23 @@
       </c>
       <c r="P10" s="6">
         <f t="shared" si="9"/>
-        <v>97646.977756784632</v>
+        <v>97647.212040473503</v>
       </c>
       <c r="Q10" s="6">
         <f t="shared" si="10"/>
-        <v>555.92838295113211</v>
+        <v>555.92971678608831</v>
       </c>
       <c r="R10" s="6">
         <f t="shared" si="1"/>
-        <v>583104.72462595219</v>
+        <v>583106.12365891051</v>
       </c>
       <c r="S10" s="6">
         <f t="shared" si="2"/>
-        <v>5112566.8674170487</v>
+        <v>5112579.6739394274</v>
       </c>
       <c r="T10" s="1">
         <f t="shared" si="5"/>
-        <v>52.357655965054391</v>
+        <v>52.357661494936785</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1311,23 +1312,23 @@
       </c>
       <c r="P11" s="6">
         <f t="shared" si="9"/>
-        <v>97091.049373833506</v>
+        <v>97091.28232368741</v>
       </c>
       <c r="Q11" s="6">
         <f t="shared" si="10"/>
-        <v>842.23677372398924</v>
+        <v>842.23879449660069</v>
       </c>
       <c r="R11" s="6">
         <f t="shared" si="1"/>
-        <v>578337.61237438105</v>
+        <v>578338.99996964145</v>
       </c>
       <c r="S11" s="6">
         <f t="shared" si="2"/>
-        <v>4529462.1427910961</v>
+        <v>4529473.550280517</v>
       </c>
       <c r="T11" s="1">
         <f t="shared" si="5"/>
-        <v>46.651696237735869</v>
+        <v>46.651701799343307</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1385,23 +1386,23 @@
       </c>
       <c r="P12" s="6">
         <f t="shared" si="9"/>
-        <v>96248.812600109522</v>
+        <v>96249.043529190807</v>
       </c>
       <c r="Q12" s="6">
         <f t="shared" si="10"/>
-        <v>1227.7137441585883</v>
+        <v>1227.7166898033122</v>
       </c>
       <c r="R12" s="6">
         <f t="shared" si="1"/>
-        <v>571356.80687986419</v>
+        <v>571358.17772612826</v>
       </c>
       <c r="S12" s="6">
         <f t="shared" si="2"/>
-        <v>3951124.530416715</v>
+        <v>3951134.5503108753</v>
       </c>
       <c r="T12" s="1">
         <f t="shared" si="5"/>
-        <v>41.051150904403144</v>
+        <v>41.05115651474042</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1459,23 +1460,23 @@
       </c>
       <c r="P13" s="6">
         <f t="shared" si="9"/>
-        <v>95021.098855950928</v>
+        <v>95021.32683938749</v>
       </c>
       <c r="Q13" s="6">
         <f t="shared" si="10"/>
-        <v>1815.1673671298095</v>
+        <v>1815.1717222477703</v>
       </c>
       <c r="R13" s="6">
         <f t="shared" si="1"/>
-        <v>561053.25630005659</v>
+        <v>561054.60242508608</v>
       </c>
       <c r="S13" s="6">
         <f t="shared" si="2"/>
-        <v>3379767.7235368509</v>
+        <v>3379776.3725847472</v>
       </c>
       <c r="T13" s="1">
         <f t="shared" si="5"/>
-        <v>35.568602807472004</v>
+        <v>35.56860849036039</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1533,23 +1534,23 @@
       </c>
       <c r="P14" s="6">
         <f t="shared" si="9"/>
-        <v>93205.931488821123</v>
+        <v>93206.155117139715</v>
       </c>
       <c r="Q14" s="6">
         <f t="shared" si="10"/>
-        <v>2716.1251790894025</v>
+        <v>2716.1316958689376</v>
       </c>
       <c r="R14" s="6">
         <f t="shared" si="1"/>
-        <v>545657.46303747979</v>
+        <v>545658.77222349355</v>
       </c>
       <c r="S14" s="6">
         <f t="shared" si="2"/>
-        <v>2818714.4672367945</v>
+        <v>2818721.7701596608</v>
       </c>
       <c r="T14" s="1">
         <f t="shared" si="5"/>
-        <v>30.241792793786562</v>
+        <v>30.241798587412443</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1607,23 +1608,23 @@
       </c>
       <c r="P15" s="6">
         <f t="shared" si="9"/>
-        <v>90489.806309731721</v>
+        <v>90490.023421270773</v>
       </c>
       <c r="Q15" s="6">
         <f t="shared" si="10"/>
-        <v>4098.6848580866235</v>
+        <v>4098.6946920316159</v>
       </c>
       <c r="R15" s="6">
         <f t="shared" si="1"/>
-        <v>522447.91356795724</v>
+        <v>522449.16706746659</v>
       </c>
       <c r="S15" s="6">
         <f t="shared" si="2"/>
-        <v>2273057.0041993149</v>
+        <v>2273062.9979361673</v>
       </c>
       <c r="T15" s="1">
         <f t="shared" si="5"/>
-        <v>25.119481374719875</v>
+        <v>25.119487342312439</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1681,23 +1682,23 @@
       </c>
       <c r="P16" s="6">
         <f t="shared" si="9"/>
-        <v>86391.1214516451</v>
+        <v>86391.328729239161</v>
       </c>
       <c r="Q16" s="6">
         <f t="shared" si="10"/>
-        <v>5928.7629884442431</v>
+        <v>5928.777213282483</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" si="1"/>
-        <v>488705.41376764938</v>
+        <v>488706.5863090225</v>
       </c>
       <c r="S16" s="6">
         <f t="shared" si="2"/>
-        <v>1750609.0906313576</v>
+        <v>1750613.8308687008</v>
       </c>
       <c r="T16" s="1">
         <f t="shared" si="5"/>
-        <v>20.26376161364232</v>
+        <v>20.263767864426946</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -1755,23 +1756,23 @@
       </c>
       <c r="P17" s="6">
         <f t="shared" si="9"/>
-        <v>80462.358463200857</v>
+        <v>80462.551515956671</v>
       </c>
       <c r="Q17" s="6">
         <f t="shared" si="10"/>
-        <v>8334.7681804038948</v>
+        <v>8334.7881779530217</v>
       </c>
       <c r="R17" s="6">
         <f t="shared" si="1"/>
-        <v>441102.80987718573</v>
+        <v>441103.86820597493</v>
       </c>
       <c r="S17" s="6">
         <f t="shared" si="2"/>
-        <v>1261903.6768637083</v>
+        <v>1261907.2445596782</v>
       </c>
       <c r="T17" s="1">
         <f t="shared" si="5"/>
-        <v>15.683155465059292</v>
+        <v>15.683162176499302</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -1829,23 +1830,23 @@
       </c>
       <c r="P18" s="6">
         <f t="shared" si="9"/>
-        <v>72127.590282796969</v>
+        <v>72127.763338003657</v>
       </c>
       <c r="Q18" s="6">
         <f t="shared" si="10"/>
-        <v>12117.065180786813</v>
+        <v>12117.094253173829</v>
       </c>
       <c r="R18" s="6">
         <f>P19*L18+P18+N18</f>
-        <v>372182.7157928478</v>
+        <v>372183.60876215284</v>
       </c>
       <c r="S18" s="6">
         <f>S19+R18</f>
-        <v>820800.86698652257</v>
+        <v>820803.37635370344</v>
       </c>
       <c r="T18" s="1">
         <f t="shared" si="5"/>
-        <v>11.379845961418322</v>
+        <v>11.379853448487948</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -1897,23 +1898,23 @@
       </c>
       <c r="P19" s="6">
         <f t="shared" si="9"/>
-        <v>60010.525102010157</v>
+        <v>60010.669084829831</v>
       </c>
       <c r="Q19" s="6">
         <f t="shared" si="10"/>
-        <v>60010.525102010157</v>
+        <v>60010.669084829831</v>
       </c>
       <c r="R19" s="12">
         <f>(3.725+0.0000625*P19)*P19</f>
-        <v>448618.15119367477</v>
+        <v>448619.7675915506</v>
       </c>
       <c r="S19" s="6">
         <f>R19</f>
-        <v>448618.15119367477</v>
+        <v>448619.7675915506</v>
       </c>
       <c r="T19" s="1">
         <f t="shared" si="5"/>
-        <v>7.4756578188756349</v>
+        <v>7.4756668178018648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>